<commit_message>
Simplify Lb_Template, Start withdraw round ID
</commit_message>
<xml_diff>
--- a/Valero Texas Open -- 2019.xlsx
+++ b/Valero Texas Open -- 2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Pools\Golf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stuff\Programming\golf_pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2722B51B-BED3-4207-96C0-10CCF9E8296D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48ED30D2-25CF-4B64-9E50-B16D55B19478}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45210" yWindow="3690" windowWidth="25845" windowHeight="17190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="3525" windowWidth="25845" windowHeight="17190" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="453">
   <si>
     <t>Thursday Total</t>
   </si>
@@ -1322,9 +1322,6 @@
     <t>J. Etulain</t>
   </si>
   <si>
-    <t>wd</t>
-  </si>
-  <si>
     <t>D.A. Points</t>
   </si>
   <si>
@@ -1407,6 +1404,12 @@
   </si>
   <si>
     <t>penalty_score</t>
+  </si>
+  <si>
+    <t>wd1</t>
+  </si>
+  <si>
+    <t>wd2</t>
   </si>
 </sst>
 </file>
@@ -1819,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2923,7 +2926,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>J2-(par_total*4)</f>
+        <f t="shared" ref="C2:C33" si="0">J2-(par_total*4)</f>
         <v>-20</v>
       </c>
       <c r="D2">
@@ -2977,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>J3-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-18</v>
       </c>
       <c r="D3">
@@ -3005,7 +3008,7 @@
         <v>67</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J66" si="0">SUM(F3:I3)</f>
+        <f t="shared" ref="J3:J66" si="1">SUM(F3:I3)</f>
         <v>270</v>
       </c>
       <c r="K3">
@@ -3031,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f>J4-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-17</v>
       </c>
       <c r="D4">
@@ -3059,7 +3062,7 @@
         <v>64</v>
       </c>
       <c r="J4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>271</v>
       </c>
       <c r="K4">
@@ -3085,7 +3088,7 @@
         <v>T4</v>
       </c>
       <c r="C5">
-        <f>J5-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-15</v>
       </c>
       <c r="D5">
@@ -3113,7 +3116,7 @@
         <v>66</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
       <c r="K5">
@@ -3139,7 +3142,7 @@
         <v>T4</v>
       </c>
       <c r="C6">
-        <f>J6-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-15</v>
       </c>
       <c r="D6">
@@ -3167,7 +3170,7 @@
         <v>72</v>
       </c>
       <c r="J6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>273</v>
       </c>
       <c r="K6">
@@ -3193,7 +3196,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>J7-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-14</v>
       </c>
       <c r="D7">
@@ -3221,7 +3224,7 @@
         <v>64</v>
       </c>
       <c r="J7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>274</v>
       </c>
       <c r="K7">
@@ -3247,7 +3250,7 @@
         <v>T7</v>
       </c>
       <c r="C8">
-        <f>J8-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D8">
@@ -3275,7 +3278,7 @@
         <v>66</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K8">
@@ -3301,7 +3304,7 @@
         <v>T7</v>
       </c>
       <c r="C9">
-        <f>J9-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D9">
@@ -3329,7 +3332,7 @@
         <v>66</v>
       </c>
       <c r="J9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K9">
@@ -3355,7 +3358,7 @@
         <v>T7</v>
       </c>
       <c r="C10">
-        <f>J10-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D10">
@@ -3383,7 +3386,7 @@
         <v>68</v>
       </c>
       <c r="J10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K10">
@@ -3409,7 +3412,7 @@
         <v>T7</v>
       </c>
       <c r="C11">
-        <f>J11-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D11">
@@ -3437,7 +3440,7 @@
         <v>70</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K11">
@@ -3463,7 +3466,7 @@
         <v>T7</v>
       </c>
       <c r="C12">
-        <f>J12-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D12">
@@ -3491,7 +3494,7 @@
         <v>70</v>
       </c>
       <c r="J12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K12">
@@ -3517,7 +3520,7 @@
         <v>T7</v>
       </c>
       <c r="C13">
-        <f>J13-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D13">
@@ -3545,7 +3548,7 @@
         <v>69</v>
       </c>
       <c r="J13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K13">
@@ -3571,7 +3574,7 @@
         <v>T7</v>
       </c>
       <c r="C14">
-        <f>J14-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
       <c r="D14">
@@ -3599,7 +3602,7 @@
         <v>71</v>
       </c>
       <c r="J14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>276</v>
       </c>
       <c r="K14">
@@ -3625,7 +3628,7 @@
         <v>T14</v>
       </c>
       <c r="C15">
-        <f>J15-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="D15">
@@ -3653,7 +3656,7 @@
         <v>66</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>277</v>
       </c>
       <c r="K15">
@@ -3679,7 +3682,7 @@
         <v>T14</v>
       </c>
       <c r="C16">
-        <f>J16-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="D16">
@@ -3707,7 +3710,7 @@
         <v>69</v>
       </c>
       <c r="J16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>277</v>
       </c>
       <c r="K16">
@@ -3733,7 +3736,7 @@
         <v>T14</v>
       </c>
       <c r="C17">
-        <f>J17-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="D17">
@@ -3761,7 +3764,7 @@
         <v>72</v>
       </c>
       <c r="J17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>277</v>
       </c>
       <c r="K17">
@@ -3787,7 +3790,7 @@
         <v>T17</v>
       </c>
       <c r="C18">
-        <f>J18-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
       <c r="D18">
@@ -3815,7 +3818,7 @@
         <v>67</v>
       </c>
       <c r="J18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
       <c r="K18">
@@ -3841,7 +3844,7 @@
         <v>T17</v>
       </c>
       <c r="C19">
-        <f>J19-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
       <c r="D19">
@@ -3869,7 +3872,7 @@
         <v>69</v>
       </c>
       <c r="J19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
       <c r="K19">
@@ -3895,7 +3898,7 @@
         <v>T17</v>
       </c>
       <c r="C20">
-        <f>J20-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
       <c r="D20">
@@ -3923,7 +3926,7 @@
         <v>70</v>
       </c>
       <c r="J20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>278</v>
       </c>
       <c r="K20">
@@ -3949,7 +3952,7 @@
         <v>T20</v>
       </c>
       <c r="C21">
-        <f>J21-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
       <c r="D21">
@@ -3977,7 +3980,7 @@
         <v>69</v>
       </c>
       <c r="J21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="K21">
@@ -4003,7 +4006,7 @@
         <v>T20</v>
       </c>
       <c r="C22">
-        <f>J22-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
       <c r="D22">
@@ -4031,7 +4034,7 @@
         <v>67</v>
       </c>
       <c r="J22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="K22">
@@ -4057,7 +4060,7 @@
         <v>T20</v>
       </c>
       <c r="C23">
-        <f>J23-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
       <c r="D23">
@@ -4085,7 +4088,7 @@
         <v>70</v>
       </c>
       <c r="J23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="K23">
@@ -4111,7 +4114,7 @@
         <v>T23</v>
       </c>
       <c r="C24">
-        <f>J24-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D24">
@@ -4139,7 +4142,7 @@
         <v>70</v>
       </c>
       <c r="J24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K24">
@@ -4165,7 +4168,7 @@
         <v>T23</v>
       </c>
       <c r="C25">
-        <f>J25-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D25">
@@ -4193,7 +4196,7 @@
         <v>70</v>
       </c>
       <c r="J25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K25">
@@ -4219,7 +4222,7 @@
         <v>T23</v>
       </c>
       <c r="C26">
-        <f>J26-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D26">
@@ -4247,7 +4250,7 @@
         <v>70</v>
       </c>
       <c r="J26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K26">
@@ -4273,7 +4276,7 @@
         <v>T23</v>
       </c>
       <c r="C27">
-        <f>J27-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D27">
@@ -4301,7 +4304,7 @@
         <v>71</v>
       </c>
       <c r="J27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K27">
@@ -4327,7 +4330,7 @@
         <v>T23</v>
       </c>
       <c r="C28">
-        <f>J28-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D28">
@@ -4355,7 +4358,7 @@
         <v>71</v>
       </c>
       <c r="J28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K28">
@@ -4381,7 +4384,7 @@
         <v>T23</v>
       </c>
       <c r="C29">
-        <f>J29-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D29">
@@ -4409,7 +4412,7 @@
         <v>71</v>
       </c>
       <c r="J29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K29">
@@ -4435,7 +4438,7 @@
         <v>T23</v>
       </c>
       <c r="C30">
-        <f>J30-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-8</v>
       </c>
       <c r="D30">
@@ -4463,7 +4466,7 @@
         <v>66</v>
       </c>
       <c r="J30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>280</v>
       </c>
       <c r="K30">
@@ -4489,7 +4492,7 @@
         <v>T30</v>
       </c>
       <c r="C31">
-        <f>J31-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="D31">
@@ -4517,7 +4520,7 @@
         <v>70</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K31">
@@ -4543,7 +4546,7 @@
         <v>T30</v>
       </c>
       <c r="C32">
-        <f>J32-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="D32">
@@ -4571,7 +4574,7 @@
         <v>70</v>
       </c>
       <c r="J32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K32">
@@ -4597,7 +4600,7 @@
         <v>T30</v>
       </c>
       <c r="C33">
-        <f>J33-(par_total*4)</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="D33">
@@ -4625,7 +4628,7 @@
         <v>72</v>
       </c>
       <c r="J33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K33">
@@ -4651,7 +4654,7 @@
         <v>T30</v>
       </c>
       <c r="C34">
-        <f>J34-(par_total*4)</f>
+        <f t="shared" ref="C34:C65" si="2">J34-(par_total*4)</f>
         <v>-7</v>
       </c>
       <c r="D34">
@@ -4679,7 +4682,7 @@
         <v>71</v>
       </c>
       <c r="J34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K34">
@@ -4705,7 +4708,7 @@
         <v>T30</v>
       </c>
       <c r="C35">
-        <f>J35-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-7</v>
       </c>
       <c r="D35">
@@ -4733,7 +4736,7 @@
         <v>73</v>
       </c>
       <c r="J35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K35">
@@ -4759,7 +4762,7 @@
         <v>T30</v>
       </c>
       <c r="C36">
-        <f>J36-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-7</v>
       </c>
       <c r="D36">
@@ -4787,7 +4790,7 @@
         <v>76</v>
       </c>
       <c r="J36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>281</v>
       </c>
       <c r="K36">
@@ -4813,7 +4816,7 @@
         <v>T36</v>
       </c>
       <c r="C37">
-        <f>J37-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D37">
@@ -4841,7 +4844,7 @@
         <v>72</v>
       </c>
       <c r="J37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K37">
@@ -4867,7 +4870,7 @@
         <v>T36</v>
       </c>
       <c r="C38">
-        <f>J38-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D38">
@@ -4895,7 +4898,7 @@
         <v>72</v>
       </c>
       <c r="J38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K38">
@@ -4921,7 +4924,7 @@
         <v>T36</v>
       </c>
       <c r="C39">
-        <f>J39-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D39">
@@ -4949,7 +4952,7 @@
         <v>72</v>
       </c>
       <c r="J39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K39">
@@ -4975,7 +4978,7 @@
         <v>T36</v>
       </c>
       <c r="C40">
-        <f>J40-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D40">
@@ -5003,7 +5006,7 @@
         <v>72</v>
       </c>
       <c r="J40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K40">
@@ -5029,7 +5032,7 @@
         <v>T36</v>
       </c>
       <c r="C41">
-        <f>J41-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D41">
@@ -5057,7 +5060,7 @@
         <v>73</v>
       </c>
       <c r="J41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K41">
@@ -5083,7 +5086,7 @@
         <v>T36</v>
       </c>
       <c r="C42">
-        <f>J42-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-6</v>
       </c>
       <c r="D42">
@@ -5111,7 +5114,7 @@
         <v>69</v>
       </c>
       <c r="J42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>282</v>
       </c>
       <c r="K42">
@@ -5137,7 +5140,7 @@
         <v>T42</v>
       </c>
       <c r="C43">
-        <f>J43-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D43">
@@ -5165,7 +5168,7 @@
         <v>73</v>
       </c>
       <c r="J43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K43">
@@ -5191,7 +5194,7 @@
         <v>T42</v>
       </c>
       <c r="C44">
-        <f>J44-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D44">
@@ -5219,7 +5222,7 @@
         <v>73</v>
       </c>
       <c r="J44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K44">
@@ -5245,7 +5248,7 @@
         <v>T42</v>
       </c>
       <c r="C45">
-        <f>J45-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D45">
@@ -5273,7 +5276,7 @@
         <v>73</v>
       </c>
       <c r="J45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K45">
@@ -5299,7 +5302,7 @@
         <v>T42</v>
       </c>
       <c r="C46">
-        <f>J46-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D46">
@@ -5327,7 +5330,7 @@
         <v>71</v>
       </c>
       <c r="J46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K46">
@@ -5353,7 +5356,7 @@
         <v>T42</v>
       </c>
       <c r="C47">
-        <f>J47-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D47">
@@ -5381,7 +5384,7 @@
         <v>71</v>
       </c>
       <c r="J47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K47">
@@ -5407,7 +5410,7 @@
         <v>T42</v>
       </c>
       <c r="C48">
-        <f>J48-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D48">
@@ -5435,7 +5438,7 @@
         <v>70</v>
       </c>
       <c r="J48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K48">
@@ -5461,7 +5464,7 @@
         <v>T42</v>
       </c>
       <c r="C49">
-        <f>J49-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D49">
@@ -5489,7 +5492,7 @@
         <v>74</v>
       </c>
       <c r="J49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K49">
@@ -5515,7 +5518,7 @@
         <v>T42</v>
       </c>
       <c r="C50">
-        <f>J50-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D50">
@@ -5543,7 +5546,7 @@
         <v>70</v>
       </c>
       <c r="J50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K50">
@@ -5569,7 +5572,7 @@
         <v>T42</v>
       </c>
       <c r="C51">
-        <f>J51-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D51">
@@ -5597,7 +5600,7 @@
         <v>69</v>
       </c>
       <c r="J51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K51">
@@ -5623,7 +5626,7 @@
         <v>T42</v>
       </c>
       <c r="C52">
-        <f>J52-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
       <c r="D52">
@@ -5651,7 +5654,7 @@
         <v>69</v>
       </c>
       <c r="J52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>283</v>
       </c>
       <c r="K52">
@@ -5677,7 +5680,7 @@
         <v>T52</v>
       </c>
       <c r="C53">
-        <f>J53-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="D53">
@@ -5705,7 +5708,7 @@
         <v>72</v>
       </c>
       <c r="J53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="K53">
@@ -5731,7 +5734,7 @@
         <v>T52</v>
       </c>
       <c r="C54">
-        <f>J54-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="D54">
@@ -5759,7 +5762,7 @@
         <v>71</v>
       </c>
       <c r="J54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="K54">
@@ -5785,7 +5788,7 @@
         <v>T52</v>
       </c>
       <c r="C55">
-        <f>J55-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="D55">
@@ -5813,7 +5816,7 @@
         <v>71</v>
       </c>
       <c r="J55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="K55">
@@ -5839,7 +5842,7 @@
         <v>T52</v>
       </c>
       <c r="C56">
-        <f>J56-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="D56">
@@ -5867,7 +5870,7 @@
         <v>70</v>
       </c>
       <c r="J56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="K56">
@@ -5893,7 +5896,7 @@
         <v>T52</v>
       </c>
       <c r="C57">
-        <f>J57-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-4</v>
       </c>
       <c r="D57">
@@ -5921,7 +5924,7 @@
         <v>70</v>
       </c>
       <c r="J57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>284</v>
       </c>
       <c r="K57">
@@ -5947,7 +5950,7 @@
         <v>T57</v>
       </c>
       <c r="C58">
-        <f>J58-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="D58">
@@ -5975,7 +5978,7 @@
         <v>73</v>
       </c>
       <c r="J58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="K58">
@@ -6001,7 +6004,7 @@
         <v>T57</v>
       </c>
       <c r="C59">
-        <f>J59-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="D59">
@@ -6029,7 +6032,7 @@
         <v>71</v>
       </c>
       <c r="J59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="K59">
@@ -6055,7 +6058,7 @@
         <v>T57</v>
       </c>
       <c r="C60">
-        <f>J60-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="D60">
@@ -6083,7 +6086,7 @@
         <v>71</v>
       </c>
       <c r="J60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="K60">
@@ -6109,7 +6112,7 @@
         <v>T57</v>
       </c>
       <c r="C61">
-        <f>J61-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-3</v>
       </c>
       <c r="D61">
@@ -6137,7 +6140,7 @@
         <v>70</v>
       </c>
       <c r="J61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="K61">
@@ -6163,7 +6166,7 @@
         <v>T61</v>
       </c>
       <c r="C62">
-        <f>J62-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="D62">
@@ -6191,7 +6194,7 @@
         <v>74</v>
       </c>
       <c r="J62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>286</v>
       </c>
       <c r="K62">
@@ -6217,7 +6220,7 @@
         <v>T61</v>
       </c>
       <c r="C63">
-        <f>J63-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-2</v>
       </c>
       <c r="D63">
@@ -6245,7 +6248,7 @@
         <v>73</v>
       </c>
       <c r="J63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>286</v>
       </c>
       <c r="K63">
@@ -6271,7 +6274,7 @@
         <v>T63</v>
       </c>
       <c r="C64">
-        <f>J64-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="D64">
@@ -6299,7 +6302,7 @@
         <v>76</v>
       </c>
       <c r="J64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287</v>
       </c>
       <c r="K64">
@@ -6325,7 +6328,7 @@
         <v>T63</v>
       </c>
       <c r="C65">
-        <f>J65-(par_total*4)</f>
+        <f t="shared" si="2"/>
         <v>-1</v>
       </c>
       <c r="D65">
@@ -6353,7 +6356,7 @@
         <v>76</v>
       </c>
       <c r="J65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287</v>
       </c>
       <c r="K65">
@@ -6379,7 +6382,7 @@
         <v>T63</v>
       </c>
       <c r="C66">
-        <f>J66-(par_total*4)</f>
+        <f t="shared" ref="C66:C97" si="3">J66-(par_total*4)</f>
         <v>-1</v>
       </c>
       <c r="D66">
@@ -6407,7 +6410,7 @@
         <v>72</v>
       </c>
       <c r="J66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287</v>
       </c>
       <c r="K66">
@@ -6433,7 +6436,7 @@
         <v>66</v>
       </c>
       <c r="C67">
-        <f>J67-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D67">
@@ -6461,7 +6464,7 @@
         <v>73</v>
       </c>
       <c r="J67">
-        <f t="shared" ref="J67:J130" si="1">SUM(F67:I67)</f>
+        <f t="shared" ref="J67:J130" si="4">SUM(F67:I67)</f>
         <v>288</v>
       </c>
       <c r="K67">
@@ -6487,7 +6490,7 @@
         <v>T67</v>
       </c>
       <c r="C68">
-        <f>J68-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D68">
@@ -6515,7 +6518,7 @@
         <v>74</v>
       </c>
       <c r="J68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>289</v>
       </c>
       <c r="K68">
@@ -6541,7 +6544,7 @@
         <v>T67</v>
       </c>
       <c r="C69">
-        <f>J69-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D69">
@@ -6569,7 +6572,7 @@
         <v>74</v>
       </c>
       <c r="J69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>289</v>
       </c>
       <c r="K69">
@@ -6595,7 +6598,7 @@
         <v>T69</v>
       </c>
       <c r="C70">
-        <f>J70-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D70">
@@ -6623,7 +6626,7 @@
         <v>80</v>
       </c>
       <c r="J70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>290</v>
       </c>
       <c r="K70">
@@ -6649,7 +6652,7 @@
         <v>T69</v>
       </c>
       <c r="C71">
-        <f>J71-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D71">
@@ -6677,7 +6680,7 @@
         <v>76</v>
       </c>
       <c r="J71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>290</v>
       </c>
       <c r="K71">
@@ -6703,7 +6706,7 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <f>J72-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D72">
@@ -6731,7 +6734,7 @@
         <v>78</v>
       </c>
       <c r="J72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>294</v>
       </c>
       <c r="K72">
@@ -6757,7 +6760,7 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <f>J73-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D73">
@@ -6785,7 +6788,7 @@
         <v>78</v>
       </c>
       <c r="J73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>294</v>
       </c>
       <c r="K73">
@@ -6811,7 +6814,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <f>J74-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D74">
@@ -6839,7 +6842,7 @@
         <v>78</v>
       </c>
       <c r="J74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>294</v>
       </c>
       <c r="K74">
@@ -6865,7 +6868,7 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <f>J75-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D75">
@@ -6893,7 +6896,7 @@
         <v>78</v>
       </c>
       <c r="J75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>294</v>
       </c>
       <c r="K75">
@@ -6919,7 +6922,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <f>J76-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D76">
@@ -6947,7 +6950,7 @@
         <v>78</v>
       </c>
       <c r="J76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>294</v>
       </c>
       <c r="K76">
@@ -6973,7 +6976,7 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <f>J77-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="D77">
@@ -7001,7 +7004,7 @@
         <v>78</v>
       </c>
       <c r="J77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>295</v>
       </c>
       <c r="K77">
@@ -7027,7 +7030,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <f>J78-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D78">
@@ -7055,7 +7058,7 @@
         <v>78</v>
       </c>
       <c r="J78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>297</v>
       </c>
       <c r="K78">
@@ -7081,7 +7084,7 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <f>J79-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D79">
@@ -7109,7 +7112,7 @@
         <v>78</v>
       </c>
       <c r="J79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>297</v>
       </c>
       <c r="K79">
@@ -7135,7 +7138,7 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <f>J80-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="D80">
@@ -7163,7 +7166,7 @@
         <v>78</v>
       </c>
       <c r="J80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>297</v>
       </c>
       <c r="K80">
@@ -7189,7 +7192,7 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <f>J81-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D81">
@@ -7217,7 +7220,7 @@
         <v>78</v>
       </c>
       <c r="J81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K81">
@@ -7243,7 +7246,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <f>J82-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D82">
@@ -7271,7 +7274,7 @@
         <v>78</v>
       </c>
       <c r="J82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K82">
@@ -7297,7 +7300,7 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <f>J83-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D83">
@@ -7325,7 +7328,7 @@
         <v>78</v>
       </c>
       <c r="J83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K83">
@@ -7351,7 +7354,7 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <f>J84-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D84">
@@ -7379,7 +7382,7 @@
         <v>78</v>
       </c>
       <c r="J84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K84">
@@ -7405,7 +7408,7 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <f>J85-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D85">
@@ -7433,7 +7436,7 @@
         <v>78</v>
       </c>
       <c r="J85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K85">
@@ -7459,7 +7462,7 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <f>J86-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D86">
@@ -7487,7 +7490,7 @@
         <v>78</v>
       </c>
       <c r="J86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K86">
@@ -7513,7 +7516,7 @@
         <v>0</v>
       </c>
       <c r="C87">
-        <f>J87-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D87">
@@ -7541,7 +7544,7 @@
         <v>78</v>
       </c>
       <c r="J87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K87">
@@ -7567,7 +7570,7 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <f>J88-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D88">
@@ -7595,7 +7598,7 @@
         <v>78</v>
       </c>
       <c r="J88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K88">
@@ -7621,7 +7624,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <f>J89-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D89">
@@ -7649,7 +7652,7 @@
         <v>78</v>
       </c>
       <c r="J89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K89">
@@ -7675,7 +7678,7 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <f>J90-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D90">
@@ -7703,7 +7706,7 @@
         <v>78</v>
       </c>
       <c r="J90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K90">
@@ -7729,7 +7732,7 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <f>J91-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D91">
@@ -7757,7 +7760,7 @@
         <v>78</v>
       </c>
       <c r="J91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K91">
@@ -7783,7 +7786,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <f>J92-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D92">
@@ -7811,7 +7814,7 @@
         <v>78</v>
       </c>
       <c r="J92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K92">
@@ -7837,7 +7840,7 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <f>J93-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D93">
@@ -7865,7 +7868,7 @@
         <v>78</v>
       </c>
       <c r="J93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K93">
@@ -7891,7 +7894,7 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <f>J94-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D94">
@@ -7919,7 +7922,7 @@
         <v>78</v>
       </c>
       <c r="J94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K94">
@@ -7945,7 +7948,7 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <f>J95-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D95">
@@ -7973,7 +7976,7 @@
         <v>78</v>
       </c>
       <c r="J95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K95">
@@ -7999,7 +8002,7 @@
         <v>0</v>
       </c>
       <c r="C96">
-        <f>J96-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D96">
@@ -8027,7 +8030,7 @@
         <v>78</v>
       </c>
       <c r="J96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K96">
@@ -8053,7 +8056,7 @@
         <v>0</v>
       </c>
       <c r="C97">
-        <f>J97-(par_total*4)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="D97">
@@ -8081,7 +8084,7 @@
         <v>78</v>
       </c>
       <c r="J97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K97">
@@ -8107,7 +8110,7 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <f>J98-(par_total*4)</f>
+        <f t="shared" ref="C98:C129" si="5">J98-(par_total*4)</f>
         <v>12</v>
       </c>
       <c r="D98">
@@ -8135,7 +8138,7 @@
         <v>78</v>
       </c>
       <c r="J98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K98">
@@ -8161,7 +8164,7 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <f>J99-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D99">
@@ -8189,7 +8192,7 @@
         <v>78</v>
       </c>
       <c r="J99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K99">
@@ -8215,7 +8218,7 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <f>J100-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D100">
@@ -8243,7 +8246,7 @@
         <v>78</v>
       </c>
       <c r="J100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K100">
@@ -8269,7 +8272,7 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <f>J101-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D101">
@@ -8297,7 +8300,7 @@
         <v>78</v>
       </c>
       <c r="J101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K101">
@@ -8323,7 +8326,7 @@
         <v>0</v>
       </c>
       <c r="C102">
-        <f>J102-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D102">
@@ -8351,7 +8354,7 @@
         <v>78</v>
       </c>
       <c r="J102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="K102">
@@ -8377,7 +8380,7 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <f>J103-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D103">
@@ -8405,7 +8408,7 @@
         <v>78</v>
       </c>
       <c r="J103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K103">
@@ -8431,7 +8434,7 @@
         <v>0</v>
       </c>
       <c r="C104">
-        <f>J104-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D104">
@@ -8459,7 +8462,7 @@
         <v>78</v>
       </c>
       <c r="J104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K104">
@@ -8485,7 +8488,7 @@
         <v>0</v>
       </c>
       <c r="C105">
-        <f>J105-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D105">
@@ -8513,7 +8516,7 @@
         <v>78</v>
       </c>
       <c r="J105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K105">
@@ -8539,7 +8542,7 @@
         <v>0</v>
       </c>
       <c r="C106">
-        <f>J106-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D106">
@@ -8567,7 +8570,7 @@
         <v>78</v>
       </c>
       <c r="J106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K106">
@@ -8593,7 +8596,7 @@
         <v>0</v>
       </c>
       <c r="C107">
-        <f>J107-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D107">
@@ -8621,7 +8624,7 @@
         <v>78</v>
       </c>
       <c r="J107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K107">
@@ -8647,7 +8650,7 @@
         <v>0</v>
       </c>
       <c r="C108">
-        <f>J108-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D108">
@@ -8675,7 +8678,7 @@
         <v>78</v>
       </c>
       <c r="J108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K108">
@@ -8701,7 +8704,7 @@
         <v>0</v>
       </c>
       <c r="C109">
-        <f>J109-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D109">
@@ -8729,7 +8732,7 @@
         <v>78</v>
       </c>
       <c r="J109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K109">
@@ -8755,7 +8758,7 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <f>J110-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D110">
@@ -8783,7 +8786,7 @@
         <v>78</v>
       </c>
       <c r="J110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K110">
@@ -8809,7 +8812,7 @@
         <v>0</v>
       </c>
       <c r="C111">
-        <f>J111-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="D111">
@@ -8837,7 +8840,7 @@
         <v>78</v>
       </c>
       <c r="J111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>301</v>
       </c>
       <c r="K111">
@@ -8863,7 +8866,7 @@
         <v>0</v>
       </c>
       <c r="C112">
-        <f>J112-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D112">
@@ -8891,7 +8894,7 @@
         <v>78</v>
       </c>
       <c r="J112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>302</v>
       </c>
       <c r="K112">
@@ -8917,7 +8920,7 @@
         <v>0</v>
       </c>
       <c r="C113">
-        <f>J113-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D113">
@@ -8945,7 +8948,7 @@
         <v>78</v>
       </c>
       <c r="J113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>302</v>
       </c>
       <c r="K113">
@@ -8971,7 +8974,7 @@
         <v>0</v>
       </c>
       <c r="C114">
-        <f>J114-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D114">
@@ -8999,7 +9002,7 @@
         <v>78</v>
       </c>
       <c r="J114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>302</v>
       </c>
       <c r="K114">
@@ -9025,7 +9028,7 @@
         <v>0</v>
       </c>
       <c r="C115">
-        <f>J115-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D115">
@@ -9053,7 +9056,7 @@
         <v>78</v>
       </c>
       <c r="J115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>302</v>
       </c>
       <c r="K115">
@@ -9079,7 +9082,7 @@
         <v>0</v>
       </c>
       <c r="C116">
-        <f>J116-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D116">
@@ -9107,7 +9110,7 @@
         <v>78</v>
       </c>
       <c r="J116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K116">
@@ -9133,7 +9136,7 @@
         <v>0</v>
       </c>
       <c r="C117">
-        <f>J117-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D117">
@@ -9161,7 +9164,7 @@
         <v>78</v>
       </c>
       <c r="J117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K117">
@@ -9187,7 +9190,7 @@
         <v>0</v>
       </c>
       <c r="C118">
-        <f>J118-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D118">
@@ -9215,7 +9218,7 @@
         <v>78</v>
       </c>
       <c r="J118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K118">
@@ -9241,7 +9244,7 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <f>J119-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D119">
@@ -9269,7 +9272,7 @@
         <v>78</v>
       </c>
       <c r="J119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K119">
@@ -9295,7 +9298,7 @@
         <v>0</v>
       </c>
       <c r="C120">
-        <f>J120-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D120">
@@ -9323,7 +9326,7 @@
         <v>78</v>
       </c>
       <c r="J120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K120">
@@ -9349,7 +9352,7 @@
         <v>0</v>
       </c>
       <c r="C121">
-        <f>J121-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D121">
@@ -9377,7 +9380,7 @@
         <v>78</v>
       </c>
       <c r="J121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K121">
@@ -9403,7 +9406,7 @@
         <v>0</v>
       </c>
       <c r="C122">
-        <f>J122-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D122">
@@ -9431,7 +9434,7 @@
         <v>78</v>
       </c>
       <c r="J122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K122">
@@ -9457,7 +9460,7 @@
         <v>0</v>
       </c>
       <c r="C123">
-        <f>J123-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D123">
@@ -9485,7 +9488,7 @@
         <v>78</v>
       </c>
       <c r="J123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K123">
@@ -9511,7 +9514,7 @@
         <v>0</v>
       </c>
       <c r="C124">
-        <f>J124-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D124">
@@ -9539,7 +9542,7 @@
         <v>78</v>
       </c>
       <c r="J124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K124">
@@ -9565,7 +9568,7 @@
         <v>0</v>
       </c>
       <c r="C125">
-        <f>J125-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="D125">
@@ -9593,7 +9596,7 @@
         <v>78</v>
       </c>
       <c r="J125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>303</v>
       </c>
       <c r="K125">
@@ -9619,7 +9622,7 @@
         <v>0</v>
       </c>
       <c r="C126">
-        <f>J126-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="D126">
@@ -9647,7 +9650,7 @@
         <v>78</v>
       </c>
       <c r="J126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>304</v>
       </c>
       <c r="K126">
@@ -9673,7 +9676,7 @@
         <v>0</v>
       </c>
       <c r="C127">
-        <f>J127-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="D127">
@@ -9701,7 +9704,7 @@
         <v>78</v>
       </c>
       <c r="J127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>304</v>
       </c>
       <c r="K127">
@@ -9727,7 +9730,7 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <f>J128-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="D128">
@@ -9755,7 +9758,7 @@
         <v>78</v>
       </c>
       <c r="J128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>304</v>
       </c>
       <c r="K128">
@@ -9781,7 +9784,7 @@
         <v>0</v>
       </c>
       <c r="C129">
-        <f>J129-(par_total*4)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="D129">
@@ -9809,7 +9812,7 @@
         <v>78</v>
       </c>
       <c r="J129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>304</v>
       </c>
       <c r="K129">
@@ -9835,7 +9838,7 @@
         <v>0</v>
       </c>
       <c r="C130">
-        <f>J130-(par_total*4)</f>
+        <f t="shared" ref="C130:C157" si="6">J130-(par_total*4)</f>
         <v>16</v>
       </c>
       <c r="D130">
@@ -9863,7 +9866,7 @@
         <v>78</v>
       </c>
       <c r="J130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>304</v>
       </c>
       <c r="K130">
@@ -9889,7 +9892,7 @@
         <v>0</v>
       </c>
       <c r="C131">
-        <f>J131-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D131">
@@ -9917,7 +9920,7 @@
         <v>78</v>
       </c>
       <c r="J131">
-        <f t="shared" ref="J131:J157" si="2">SUM(F131:I131)</f>
+        <f t="shared" ref="J131:J157" si="7">SUM(F131:I131)</f>
         <v>305</v>
       </c>
       <c r="K131">
@@ -9943,7 +9946,7 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <f>J132-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D132">
@@ -9971,7 +9974,7 @@
         <v>78</v>
       </c>
       <c r="J132">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="K132">
@@ -9997,7 +10000,7 @@
         <v>0</v>
       </c>
       <c r="C133">
-        <f>J133-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D133">
@@ -10025,7 +10028,7 @@
         <v>78</v>
       </c>
       <c r="J133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="K133">
@@ -10051,7 +10054,7 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <f>J134-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D134">
@@ -10079,7 +10082,7 @@
         <v>78</v>
       </c>
       <c r="J134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="K134">
@@ -10105,7 +10108,7 @@
         <v>0</v>
       </c>
       <c r="C135">
-        <f>J135-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D135">
@@ -10133,7 +10136,7 @@
         <v>78</v>
       </c>
       <c r="J135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="K135">
@@ -10159,7 +10162,7 @@
         <v>0</v>
       </c>
       <c r="C136">
-        <f>J136-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="D136">
@@ -10187,7 +10190,7 @@
         <v>78</v>
       </c>
       <c r="J136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>305</v>
       </c>
       <c r="K136">
@@ -10213,7 +10216,7 @@
         <v>0</v>
       </c>
       <c r="C137">
-        <f>J137-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="D137">
@@ -10241,7 +10244,7 @@
         <v>78</v>
       </c>
       <c r="J137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="K137">
@@ -10267,7 +10270,7 @@
         <v>0</v>
       </c>
       <c r="C138">
-        <f>J138-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="D138">
@@ -10295,7 +10298,7 @@
         <v>78</v>
       </c>
       <c r="J138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>306</v>
       </c>
       <c r="K138">
@@ -10321,7 +10324,7 @@
         <v>0</v>
       </c>
       <c r="C139">
-        <f>J139-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="D139">
@@ -10349,7 +10352,7 @@
         <v>78</v>
       </c>
       <c r="J139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>307</v>
       </c>
       <c r="K139">
@@ -10375,7 +10378,7 @@
         <v>0</v>
       </c>
       <c r="C140">
-        <f>J140-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D140">
@@ -10403,7 +10406,7 @@
         <v>78</v>
       </c>
       <c r="J140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>308</v>
       </c>
       <c r="K140">
@@ -10429,7 +10432,7 @@
         <v>0</v>
       </c>
       <c r="C141">
-        <f>J141-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="D141">
@@ -10457,7 +10460,7 @@
         <v>78</v>
       </c>
       <c r="J141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>308</v>
       </c>
       <c r="K141">
@@ -10483,7 +10486,7 @@
         <v>0</v>
       </c>
       <c r="C142">
-        <f>J142-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="D142">
@@ -10511,7 +10514,7 @@
         <v>78</v>
       </c>
       <c r="J142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>309</v>
       </c>
       <c r="K142">
@@ -10537,7 +10540,7 @@
         <v>0</v>
       </c>
       <c r="C143">
-        <f>J143-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="D143">
@@ -10565,7 +10568,7 @@
         <v>78</v>
       </c>
       <c r="J143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>312</v>
       </c>
       <c r="K143">
@@ -10574,7 +10577,7 @@
       </c>
       <c r="L143" t="str">
         <f>INDEX(player_data,MATCH($A143,'Raw Data'!$B$1:$B$157,0),MATCH(L$1,'Raw Data'!$A$1:$R$1,0))</f>
-        <v>wd</v>
+        <v>wd2</v>
       </c>
       <c r="M143">
         <f>INDEX(player_data,MATCH($A143,'Raw Data'!$B$1:$B$157,0),MATCH(M$1,'Raw Data'!$A$1:$R$1,0))</f>
@@ -10591,7 +10594,7 @@
         <v>0</v>
       </c>
       <c r="C144">
-        <f>J144-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="D144">
@@ -10619,7 +10622,7 @@
         <v>78</v>
       </c>
       <c r="J144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>312</v>
       </c>
       <c r="K144">
@@ -10628,7 +10631,7 @@
       </c>
       <c r="L144" t="str">
         <f>INDEX(player_data,MATCH($A144,'Raw Data'!$B$1:$B$157,0),MATCH(L$1,'Raw Data'!$A$1:$R$1,0))</f>
-        <v>wd</v>
+        <v>wd1</v>
       </c>
       <c r="M144">
         <f>INDEX(player_data,MATCH($A144,'Raw Data'!$B$1:$B$157,0),MATCH(M$1,'Raw Data'!$A$1:$R$1,0))</f>
@@ -10645,7 +10648,7 @@
         <v>0</v>
       </c>
       <c r="C145">
-        <f>J145-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="D145">
@@ -10673,7 +10676,7 @@
         <v>78</v>
       </c>
       <c r="J145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>312</v>
       </c>
       <c r="K145">
@@ -10682,7 +10685,7 @@
       </c>
       <c r="L145" t="str">
         <f>INDEX(player_data,MATCH($A145,'Raw Data'!$B$1:$B$157,0),MATCH(L$1,'Raw Data'!$A$1:$R$1,0))</f>
-        <v>wd</v>
+        <v>wd1</v>
       </c>
       <c r="M145">
         <f>INDEX(player_data,MATCH($A145,'Raw Data'!$B$1:$B$157,0),MATCH(M$1,'Raw Data'!$A$1:$R$1,0))</f>
@@ -10699,7 +10702,7 @@
         <v>#N/A</v>
       </c>
       <c r="C146" t="e">
-        <f>J146-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D146" t="e">
@@ -10727,7 +10730,7 @@
         <v>#N/A</v>
       </c>
       <c r="J146" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K146" t="e">
@@ -10753,7 +10756,7 @@
         <v>#N/A</v>
       </c>
       <c r="C147" t="e">
-        <f>J147-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D147" t="e">
@@ -10781,7 +10784,7 @@
         <v>#N/A</v>
       </c>
       <c r="J147" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K147" t="e">
@@ -10807,7 +10810,7 @@
         <v>#N/A</v>
       </c>
       <c r="C148" t="e">
-        <f>J148-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D148" t="e">
@@ -10835,7 +10838,7 @@
         <v>#N/A</v>
       </c>
       <c r="J148" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K148" t="e">
@@ -10861,7 +10864,7 @@
         <v>#N/A</v>
       </c>
       <c r="C149" t="e">
-        <f>J149-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D149" t="e">
@@ -10889,7 +10892,7 @@
         <v>#N/A</v>
       </c>
       <c r="J149" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K149" t="e">
@@ -10915,7 +10918,7 @@
         <v>#N/A</v>
       </c>
       <c r="C150" t="e">
-        <f>J150-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D150" t="e">
@@ -10943,7 +10946,7 @@
         <v>#N/A</v>
       </c>
       <c r="J150" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K150" t="e">
@@ -10969,7 +10972,7 @@
         <v>#N/A</v>
       </c>
       <c r="C151" t="e">
-        <f>J151-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D151" t="e">
@@ -10997,7 +11000,7 @@
         <v>#N/A</v>
       </c>
       <c r="J151" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K151" t="e">
@@ -11023,7 +11026,7 @@
         <v>#N/A</v>
       </c>
       <c r="C152" t="e">
-        <f>J152-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D152" t="e">
@@ -11051,7 +11054,7 @@
         <v>#N/A</v>
       </c>
       <c r="J152" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K152" t="e">
@@ -11077,7 +11080,7 @@
         <v>#N/A</v>
       </c>
       <c r="C153" t="e">
-        <f>J153-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D153" t="e">
@@ -11105,7 +11108,7 @@
         <v>#N/A</v>
       </c>
       <c r="J153" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K153" t="e">
@@ -11131,7 +11134,7 @@
         <v>#N/A</v>
       </c>
       <c r="C154" t="e">
-        <f>J154-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D154" t="e">
@@ -11159,7 +11162,7 @@
         <v>#N/A</v>
       </c>
       <c r="J154" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K154" t="e">
@@ -11185,7 +11188,7 @@
         <v>#N/A</v>
       </c>
       <c r="C155" t="e">
-        <f>J155-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D155" t="e">
@@ -11213,7 +11216,7 @@
         <v>#N/A</v>
       </c>
       <c r="J155" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K155" t="e">
@@ -11239,7 +11242,7 @@
         <v>#N/A</v>
       </c>
       <c r="C156" t="e">
-        <f>J156-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D156" t="e">
@@ -11267,7 +11270,7 @@
         <v>#N/A</v>
       </c>
       <c r="J156" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K156" t="e">
@@ -11293,7 +11296,7 @@
         <v>#N/A</v>
       </c>
       <c r="C157" t="e">
-        <f>J157-(par_total*4)</f>
+        <f t="shared" si="6"/>
         <v>#N/A</v>
       </c>
       <c r="D157" t="e">
@@ -11321,7 +11324,7 @@
         <v>#N/A</v>
       </c>
       <c r="J157" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#N/A</v>
       </c>
       <c r="K157" t="e">
@@ -11346,8 +11349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="B106" workbookViewId="0">
+      <selection activeCell="S136" sqref="S136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11362,7 +11365,7 @@
     <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17880,7 +17883,7 @@
         <v>70</v>
       </c>
       <c r="M143" t="s">
-        <v>423</v>
+        <v>452</v>
       </c>
       <c r="N143">
         <v>4</v>
@@ -17894,11 +17897,11 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>423</v>
+      </c>
+      <c r="B144" t="s">
         <v>424</v>
       </c>
-      <c r="B144" t="s">
-        <v>425</v>
-      </c>
       <c r="G144">
         <v>78</v>
       </c>
@@ -17915,7 +17918,7 @@
         <v>78</v>
       </c>
       <c r="M144" t="s">
-        <v>423</v>
+        <v>451</v>
       </c>
       <c r="O144" t="s">
         <v>72</v>
@@ -17926,11 +17929,11 @@
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>425</v>
+      </c>
+      <c r="B145" t="s">
         <v>426</v>
       </c>
-      <c r="B145" t="s">
-        <v>427</v>
-      </c>
       <c r="G145">
         <v>78</v>
       </c>
@@ -17944,7 +17947,7 @@
         <v>78</v>
       </c>
       <c r="M145" t="s">
-        <v>423</v>
+        <v>451</v>
       </c>
       <c r="N145">
         <v>9</v>
@@ -17973,39 +17976,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" t="s">
         <v>428</v>
-      </c>
-      <c r="B1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B2" t="s">
         <v>430</v>
-      </c>
-      <c r="B2" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B3" t="s">
         <v>432</v>
-      </c>
-      <c r="B3" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B4" t="s">
         <v>434</v>
-      </c>
-      <c r="B4" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
@@ -18013,7 +18016,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
@@ -18029,55 +18032,55 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>437</v>
+      </c>
+      <c r="B8" t="s">
         <v>438</v>
-      </c>
-      <c r="B8" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B9" t="s">
         <v>440</v>
-      </c>
-      <c r="B9" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>441</v>
+      </c>
+      <c r="B10" t="s">
         <v>442</v>
-      </c>
-      <c r="B10" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>443</v>
+      </c>
+      <c r="B11" t="s">
         <v>444</v>
-      </c>
-      <c r="B11" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13" t="s">
         <v>447</v>
-      </c>
-      <c r="B13" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B14">
         <v>80</v>
@@ -18085,7 +18088,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B15">
         <v>-1</v>
@@ -18093,7 +18096,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B16">
         <v>78</v>

</xml_diff>